<commit_message>
Till login All Cases
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/Data.xlsx
+++ b/src/main/java/utilities/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosh\Downloads\SSP\src\main\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8A9F03-61A2-459A-807C-28D28CDEF006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FFB542-F3B1-4747-9E31-E11A01C25D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{23862B7D-6AF9-4126-A351-97AB6D368D63}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>ipmcloud@200#</t>
   </si>
   <si>
-    <t>abchdhd</t>
-  </si>
-  <si>
     <t>wrongUsername</t>
   </si>
   <si>
@@ -81,7 +78,10 @@
     <t>sdfdsf</t>
   </si>
   <si>
-    <t>abchdhd@sfsd.dfd</t>
+    <t>adas</t>
+  </si>
+  <si>
+    <t>asdasd</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,13 +490,14 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{FF55847D-1AA7-484B-B5A8-DA9DC27E7E7D}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{4576D2A2-1974-42CA-8FDB-8CD724C6C0E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -507,7 +508,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,18 +529,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7B179779-E61D-4438-BF9E-9949BC527325}"/>
+    <hyperlink ref="B2" r:id="rId1" display="test1@vipl.com" xr:uid="{E4028C5E-8590-4760-82AD-183CA48DD8BD}"/>
+    <hyperlink ref="C2" r:id="rId2" display="ipmcloud@200#" xr:uid="{C7133945-B6E2-4341-AC2A-25CAAE769774}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -558,16 +560,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -575,10 +577,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -607,16 +609,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -624,16 +626,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -656,16 +658,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -673,10 +675,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>

</xml_diff>